<commit_message>
update sheet with scopus
</commit_message>
<xml_diff>
--- a/cities_query_v3.xlsx
+++ b/cities_query_v3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="query" sheetId="1" r:id="rId1"/>
     <sheet name="old queries" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Search string</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t xml:space="preserve">TS = (("emissions" OR "CO2" OR "carbon" OR "GHG" OR "greenhouse gas") NEAR/1 ("trading" OR "tax" OR "control" OR "regulation") NEAR/3 ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan"))  </t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Scopus</t>
   </si>
 </sst>
 </file>
@@ -202,16 +208,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -227,9 +234,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,9 +274,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,7 +346,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,21 +520,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,275 +543,296 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(B2,"TS = ","TITLE-ABS-KEY"),"NEAR/","W/")</f>
+        <v>TITLE-ABS-KEY(("bus" OR "metro" OR "subway" OR "train" OR "light rail" OR "heavy rail" OR "tram" OR "railway") AND ("transport*" OR "traffic" OR "commut*" OR "travel*") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") W/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*"))))</v>
+      </c>
+      <c r="D2">
         <v>1220</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0.84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1775</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>247</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>127</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>256</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1095</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>CONCATENATE("(",B2,")","OR","(",B3,")","OR","(",B4,")","OR","(",B5,")","OR","(",B6,")","OR","(",B7,")")</f>
+        <v>(TS = (("bus" OR "metro" OR "subway" OR "train" OR "light rail" OR "heavy rail" OR "tram" OR "railway") AND ("transport*" OR "traffic" OR "commut*" OR "travel*") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))))OR(TS = (("public" NEAR/3 ("transit" OR "transport*") OR ("mass" OR "rapid") NEAR/3 "transit") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))) NOT TS = "cell")OR(TS = (("active travel" OR "modal shift" OR "park and ride" OR "car sharing" OR "bicycle sharing" OR ("intermodal" AND ("travel" OR "transport") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan"))) AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))))OR(TS = (("electric" NEAR/1 ("car" OR "vehicle" OR "taxi")) AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))))OR(TS = (("bicycle" OR "pedestrian*" OR "walking" OR "cycling" OR "rickshaw*") NEAR/2 ("infrastructure*" OR "path" OR "paths" OR "trail*" OR "network" OR "route*" OR "corridor*" OR "lane*") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) NOT TS = "evacuation")OR(TS = (("congestion" OR "parking") NEAR/3 ("charg*" OR "tax" OR "pric*" OR "policy") AND ("transport*" OR "traffic" OR "vehicle" OR "car" OR "travel" OR "urban")) OR TS = "parking management")</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8">
+        <v>3942</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="D11">
         <v>826</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="D12">
         <v>229</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
+      <c r="D13">
         <v>924</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C13">
+      <c r="D14">
         <v>279</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="D17">
         <v>1093</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E17" s="2">
         <v>0.96</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
+      <c r="D18">
         <v>225</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E18" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="C20">
+      <c r="D21">
         <v>36</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E21" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="C21">
+      <c r="D22">
         <v>567</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E22" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C22">
+      <c r="D23">
         <v>38</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E23" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C23">
+      <c r="D24">
         <v>44</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E24" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" t="str">
-        <f>CONCATENATE("(",B2," OR ",B3," OR ",B4," OR ",B5," OR ",B6," OR ",B7," OR ",B10," OR ",B11," OR ",B12," OR ",B13," OR ",B16," OR ",B17," OR ",B20," OR ",B21," OR ",B22," OR ",B23,")",B25)</f>
+      <c r="B28" t="str">
+        <f>CONCATENATE("(",B2," OR ",B3," OR ",B4," OR ",B5," OR ",B6," OR ",B7," OR ",B11," OR ",B12," OR ",B13," OR ",B14," OR ",B17," OR ",B18," OR ",B21," OR ",B22," OR ",B23," OR ",B24,")",B26)</f>
         <v>(TS = (("bus" OR "metro" OR "subway" OR "train" OR "light rail" OR "heavy rail" OR "tram" OR "railway") AND ("transport*" OR "traffic" OR "commut*" OR "travel*") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))) OR TS = (("public" NEAR/3 ("transit" OR "transport*") OR ("mass" OR "rapid") NEAR/3 "transit") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))) NOT TS = "cell" OR TS = (("active travel" OR "modal shift" OR "park and ride" OR "car sharing" OR "bicycle sharing" OR ("intermodal" AND ("travel" OR "transport") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan"))) AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) OR TS = (("electric" NEAR/1 ("car" OR "vehicle" OR "taxi")) AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR "pricing" OR "planning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR ("information campaign" OR "marketing" OR "participatory" OR "public awareness" OR "education" OR "cooperation" OR "labels" OR "certifi*")))) OR TS = (("bicycle" OR "pedestrian*" OR "walking" OR "cycling" OR "rickshaw*") NEAR/2 ("infrastructure*" OR "path" OR "paths" OR "trail*" OR "network" OR "route*" OR "corridor*" OR "lane*") AND (("provision*" OR "subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) NOT TS = "evacuation" OR TS = (("congestion" OR "parking") NEAR/3 ("charg*" OR "tax" OR "pric*" OR "policy") AND ("transport*" OR "traffic" OR "vehicle" OR "car" OR "travel" OR "urban")) OR TS = "parking management" OR TS = ((“heating” OR “cooling” OR “thermal comfort” OR “air condition*” OR “thermostat”) AND ((“energy” OR “carbon” OR “CO2” OR “material*”) NEAR/3 (“saving*” OR “conservation” OR “perform*” OR “efficiency” )) AND ("building*" OR "occupant*") AND ("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*"))) NOT TS = "thermal regulation" OR TS = ((“lighting” OR “appliances” OR “refrigerat*” OR “cooking” OR "electrical device*") AND ((“energy” OR “carbon” OR “CO2” OR “material*”) NEAR/3 (“saving*” OR “conservation” OR “perform*” OR “efficiency” )) AND ("building*" OR "occupant*") AND ("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*"))) OR TS = ((“consumption” OR “behavior* change” OR “lifestyle” OR “sufficiency” OR “rebound”) AND ((“energy” OR “carbon” OR “CO2” OR “material*”) NEAR/3 (“saving*” OR “conservation” OR “perform*” OR “efficiency” )) AND ("building*" OR "occupant*") AND ("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*"))) OR TS = (("cool roofs" OR "green roofs" OR "passive house" OR "net zero" OR "mixed mode" OR "zero energy" OR "green building") AND ((“energy” OR “carbon” OR “CO2” OR “material*”) NEAR/3 (“saving*” OR “conservation” OR “perform*” OR “efficiency” )) AND ("building*" OR “occupant*”) AND (("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) OR TS = (("biological treatment" OR ("waste" OR "landfill") NEAR/3 ("management" OR "prevention")) AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan") AND (("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) OR TS = ((("household*" OR "residential" OR "business*" OR "municipal" OR "council" OR "metropolitan") NEAR/3 (“recycling” OR “composting”)) AND (("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) NOT TS="revenue recycling" OR TS = (("lock-in" OR "path dependen*" OR "development path") AND ("infrastructur*") AND ("urban*" OR "building*" OR "municipal" OR "city" OR "cities") AND (("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) OR TS = ((“urban form” OR “compact city” OR "dense city" OR (“low-carbon” AND “urban” AND “transition”) OR “transit-oriented development” OR “integrated land use and transport planning” OR “green infrastructure”) AND (("subsid*" OR "incentive*" OR "grant*" OR "regulat*" OR "governance" OR "codes" OR "standards" OR "tax*" OR "compliance" OR "zoning" OR (("public" OR "state" OR "government" OR "infrastructure") NEAR/3 ("investment*" OR "procurement" OR "financ*")) OR (“information campaign” OR “marketing” OR “participatory” OR “public awareness” OR “education” OR “cooperation” OR “labels” OR "certifi*")))) OR TS = (("emissions" OR "CO2" OR "carbon" OR "GHG" OR "greenhouse gas") NEAR/1 ("trading" OR "tax" OR "control" OR "regulation") NEAR/3 ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan"))   OR TS = (("climate" NEAR/3 "plan") AND ("urban*" OR "municipal" OR "city" OR "cities" OR "metropolitan"))) NOT TS = ("TRAM-34" OR "taxa" OR "subsidence" OR "ataxia")</v>
       </c>
-      <c r="C27">
+      <c r="D28">
         <v>7166</v>
       </c>
     </row>
@@ -821,7 +850,7 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>